<commit_message>
Mise à jour TO DO et création des variables relatives aux temps.
</commit_message>
<xml_diff>
--- a/infos_variables.xlsx
+++ b/infos_variables.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\telemaque\users\CEPE-S1-01\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\telemaque\users\CEPE-S1-01\Bureau\NBA_CEPE_2018_KB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13560"/>
   </bookViews>
   <sheets>
-    <sheet name="source_kb_shots,csv" sheetId="1" r:id="rId1"/>
+    <sheet name="source_kb_shots.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -552,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mise à disposition de kb_analyse.csv
</commit_message>
<xml_diff>
--- a/infos_variables.xlsx
+++ b/infos_variables.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\telemaque\users\CEPE-S1-01\Bureau\NBA_CEPE_2018_KB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13560"/>
   </bookViews>
   <sheets>
     <sheet name="source_kb_shots.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>action_type</t>
   </si>
@@ -262,13 +267,73 @@
   </si>
   <si>
     <t>Nombre de jours par rapport au dernier match (blocage avec un max à 15)</t>
+  </si>
+  <si>
+    <t>boo_premier_shot_qt</t>
+  </si>
+  <si>
+    <t>Booléen premier shot de KB du QT</t>
+  </si>
+  <si>
+    <t>boo_dernier_shot_qt</t>
+  </si>
+  <si>
+    <t>boo_premier_shot_match</t>
+  </si>
+  <si>
+    <t>boo_dernier_shot_match</t>
+  </si>
+  <si>
+    <t>Booléen dernier shot de KB du QT</t>
+  </si>
+  <si>
+    <t>Booléen premier shot de KB du match</t>
+  </si>
+  <si>
+    <t>Booléen dernier shot de KB du match</t>
+  </si>
+  <si>
+    <t>temps_dernier_shot</t>
+  </si>
+  <si>
+    <t>temps_prochain_shot</t>
+  </si>
+  <si>
+    <t>Temps en seconde depuis le dernier shot (si premier shot du QT on met 12*60=720 secondes</t>
+  </si>
+  <si>
+    <t>Temps en seconde avat le prochain shot (si dernier shot du QT on met 12*60=720 secondes</t>
+  </si>
+  <si>
+    <t>nb_shot_qt</t>
+  </si>
+  <si>
+    <t>intensite_shot_qt</t>
+  </si>
+  <si>
+    <t>Nombre de shot pris par KB au total dans le QT</t>
+  </si>
+  <si>
+    <t>Intensité des shots pris par KB sur ce QT (nombre de shot dans le QT dvisié par la durée du QT)</t>
+  </si>
+  <si>
+    <t>nb_shot_match</t>
+  </si>
+  <si>
+    <t>intensite_shot_match</t>
+  </si>
+  <si>
+    <t>Nombre de shot pris par KB au total dans le match</t>
+  </si>
+  <si>
+    <t>Intensité des shots pris par KB sur ce match (nombre de shot dans le match dvisié par la durée du match)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,35 +682,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="119.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -656,7 +721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -667,7 +732,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -678,7 +743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -689,7 +754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -700,7 +765,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -711,7 +776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -722,7 +787,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -733,7 +798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -744,7 +809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -755,7 +820,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -766,7 +831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -777,7 +842,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -788,7 +853,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -799,7 +864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -810,7 +875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -821,7 +886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -832,7 +897,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -843,7 +908,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -854,7 +919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -865,7 +930,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -876,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -887,7 +952,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -898,7 +963,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -909,7 +974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -920,7 +985,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -931,7 +996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>54</v>
       </c>
@@ -939,7 +1004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>55</v>
       </c>
@@ -947,7 +1012,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>57</v>
       </c>
@@ -955,7 +1020,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>59</v>
       </c>
@@ -963,7 +1028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>62</v>
       </c>
@@ -971,7 +1036,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>64</v>
       </c>
@@ -979,7 +1044,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>65</v>
       </c>
@@ -987,7 +1052,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>66</v>
       </c>
@@ -995,7 +1060,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>70</v>
       </c>
@@ -1003,7 +1068,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>72</v>
       </c>
@@ -1011,7 +1076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>73</v>
       </c>
@@ -1019,7 +1084,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>75</v>
       </c>
@@ -1027,7 +1092,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>77</v>
       </c>
@@ -1035,12 +1100,92 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>78</v>
       </c>
       <c r="C42" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJ 1er mai (XGboost, modèles "light", "prévision", "full" et proposition de plan pour la présentation)
</commit_message>
<xml_diff>
--- a/infos_variables.xlsx
+++ b/infos_variables.xlsx
@@ -905,7 +905,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -929,8 +929,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -967,6 +974,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -995,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,9 +1050,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1030,6 +1064,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1303,7 +1361,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1313,10 +1371,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1328,11 +1386,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1341,7 +1399,7 @@
       <c r="B2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1352,7 +1410,7 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1363,7 +1421,7 @@
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1374,7 +1432,7 @@
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1385,7 +1443,7 @@
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1396,7 +1454,7 @@
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1407,7 +1465,7 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1418,7 +1476,7 @@
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1429,7 +1487,7 @@
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1440,7 +1498,7 @@
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1451,7 +1509,7 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1462,7 +1520,7 @@
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>186</v>
       </c>
     </row>
@@ -1473,7 +1531,7 @@
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1484,7 +1542,7 @@
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1495,7 +1553,7 @@
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1506,7 +1564,7 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1517,7 +1575,7 @@
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1528,7 +1586,7 @@
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1539,7 +1597,7 @@
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1550,7 +1608,7 @@
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1561,7 +1619,7 @@
       <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1572,7 +1630,7 @@
       <c r="B23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1583,7 +1641,7 @@
       <c r="B24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1594,7 +1652,7 @@
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1605,7 +1663,7 @@
       <c r="B26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1616,7 +1674,7 @@
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1635,7 +1693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1647,11 +1705,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1660,1470 +1718,1470 @@
       <c r="B2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="3">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="3">
+      <c r="A18" s="12">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3">
+      <c r="A19" s="12">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="3">
+      <c r="A20" s="12">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="3">
+      <c r="A21" s="14">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="3">
+      <c r="A22" s="14">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="3">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="3">
+      <c r="A24" s="14">
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="3">
+      <c r="A25" s="16">
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="3">
+      <c r="A26" s="14">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="3">
+      <c r="A27" s="16">
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="3">
+      <c r="A28" s="16">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="3">
+      <c r="A29" s="16">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="3">
+      <c r="A30" s="16">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="3">
+      <c r="A31" s="16">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="3">
+      <c r="A32" s="14">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="3">
+      <c r="A33" s="17">
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="3">
+      <c r="A34" s="17">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="3">
+      <c r="A35" s="14">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="3">
+      <c r="A36" s="14">
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="3">
+      <c r="A37" s="14">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="3">
+      <c r="A38" s="14">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="3">
+      <c r="A39" s="17">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="3">
+      <c r="A40" s="17">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="3">
+      <c r="A41" s="14">
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="3">
+      <c r="A42" s="14">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="3">
+      <c r="A43" s="14">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="3">
+      <c r="A44" s="14">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="3">
+      <c r="A45" s="14">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="3">
+      <c r="A46" s="14">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="3">
+      <c r="A47" s="14">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="8" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="3">
+      <c r="A48" s="14">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="8" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="3">
+      <c r="A49" s="16">
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="8" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="3">
+      <c r="A50" s="16">
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="3">
+      <c r="A51" s="16">
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="8" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="3">
+      <c r="A52" s="16">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="8" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="3">
+      <c r="A53" s="16">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="8" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="3">
+      <c r="A54" s="14">
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="8" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="3">
+      <c r="A55" s="14">
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="3">
+      <c r="A56" s="14">
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="8" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="3">
+      <c r="A57" s="14">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="8" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="3">
+      <c r="A58" s="14">
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="8" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="3">
+      <c r="A59" s="16">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="3">
+      <c r="A60" s="16">
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="3">
+      <c r="A61" s="16">
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="8" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="3">
+      <c r="A62" s="16">
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="8" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="3">
+      <c r="A63" s="16">
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="8" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="3">
+      <c r="A64" s="12">
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="3">
+      <c r="A65" s="12">
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="3">
+      <c r="A66" s="12">
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="8" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="3">
+      <c r="A67" s="12">
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="3">
+      <c r="A68" s="12">
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="3">
+      <c r="A69" s="12">
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="3">
+      <c r="A70" s="12">
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="3">
+      <c r="A71" s="12">
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="3">
+      <c r="A72" s="12">
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="3">
+      <c r="A73" s="5">
         <v>71</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="3">
+      <c r="A74" s="5">
         <v>72</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="10" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="3">
+      <c r="A75" s="14">
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="8" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="3">
+      <c r="A76" s="13">
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="8" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="3">
+      <c r="A77" s="16">
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="8" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="3">
+      <c r="A78" s="14">
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="8" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="3">
+      <c r="A79" s="13">
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="8" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="3">
+      <c r="A80" s="16">
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="8" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="3">
+      <c r="A81" s="14">
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="8" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="3">
+      <c r="A82" s="16">
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="8" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="3">
+      <c r="A83" s="14">
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="8" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="3">
+      <c r="A84" s="17">
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="8" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="3">
+      <c r="A85" s="16">
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C85" s="9" t="s">
+      <c r="C85" s="8" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="3">
+      <c r="A86" s="17">
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="8" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="3">
+      <c r="A87" s="14">
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C87" s="8" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="3">
+      <c r="A88" s="14">
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="8" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="3">
+      <c r="A89" s="14">
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="8" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="3">
+      <c r="A90" s="17">
         <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C90" s="8" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="3">
+      <c r="A91" s="16">
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="8" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="3">
+      <c r="A92" s="17">
         <v>90</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="8" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="3">
+      <c r="A93" s="14">
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="C93" s="8" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="3">
+      <c r="A94" s="14">
         <v>92</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="8" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="3">
+      <c r="A95" s="14">
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="8" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="3">
+      <c r="A96" s="17">
         <v>94</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="8" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="3">
+      <c r="A97" s="16">
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="8" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="3">
+      <c r="A98" s="17">
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="8" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="3">
+      <c r="A99" s="14">
         <v>97</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="8" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="3">
+      <c r="A100" s="14">
         <v>98</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="8" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="3">
+      <c r="A101" s="14">
         <v>99</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="8" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="3">
+      <c r="A102" s="16">
         <v>100</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="3">
+      <c r="A103" s="16">
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C103" s="9" t="s">
+      <c r="C103" s="8" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="3">
+      <c r="A104" s="16">
         <v>102</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="8" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="3">
+      <c r="A105" s="14">
         <v>103</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C105" s="9" t="s">
+      <c r="C105" s="8" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="3">
+      <c r="A106" s="14">
         <v>104</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="8" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="3">
+      <c r="A107" s="14">
         <v>105</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C107" s="9" t="s">
+      <c r="C107" s="8" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="3">
+      <c r="A108" s="16">
         <v>106</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="8" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="3">
+      <c r="A109" s="16">
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C109" s="9" t="s">
+      <c r="C109" s="8" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="3">
+      <c r="A110" s="16">
         <v>108</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C110" s="9" t="s">
+      <c r="C110" s="8" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="3">
+      <c r="A111" s="14">
         <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C111" s="9" t="s">
+      <c r="C111" s="8" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="3">
+      <c r="A112" s="14">
         <v>110</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C112" s="9" t="s">
+      <c r="C112" s="8" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="3">
+      <c r="A113" s="14">
         <v>111</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C113" s="9" t="s">
+      <c r="C113" s="8" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="3">
+      <c r="A114" s="16">
         <v>112</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C114" s="9" t="s">
+      <c r="C114" s="8" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="3">
+      <c r="A115" s="14">
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C115" s="9" t="s">
+      <c r="C115" s="8" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="3">
+      <c r="A116" s="16">
         <v>114</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="8" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="3">
+      <c r="A117" s="14">
         <v>115</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C117" s="9" t="s">
+      <c r="C117" s="8" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="3">
+      <c r="A118" s="16">
         <v>116</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="8" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="3">
+      <c r="A119" s="14">
         <v>117</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C119" s="9" t="s">
+      <c r="C119" s="8" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="3">
+      <c r="A120" s="16">
         <v>118</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="8" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="3">
+      <c r="A121" s="14">
         <v>119</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C121" s="9" t="s">
+      <c r="C121" s="8" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="3">
+      <c r="A122" s="16">
         <v>120</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="8" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="3">
+      <c r="A123" s="14">
         <v>121</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C123" s="9" t="s">
+      <c r="C123" s="8" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="3">
+      <c r="A124" s="17">
         <v>122</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C124" s="9" t="s">
+      <c r="C124" s="8" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="3">
+      <c r="A125" s="14">
         <v>123</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C125" s="9" t="s">
+      <c r="C125" s="8" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="3">
+      <c r="A126" s="17">
         <v>124</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C126" s="9" t="s">
+      <c r="C126" s="8" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="3">
+      <c r="A127" s="14">
         <v>125</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C127" s="9" t="s">
+      <c r="C127" s="8" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="3">
+      <c r="A128" s="17">
         <v>126</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C128" s="9" t="s">
+      <c r="C128" s="8" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="3">
+      <c r="A129" s="14">
         <v>127</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C129" s="9" t="s">
+      <c r="C129" s="8" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="3">
+      <c r="A130" s="17">
         <v>128</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C130" s="9" t="s">
+      <c r="C130" s="8" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="3">
+      <c r="A131" s="17">
         <v>129</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C131" s="9" t="s">
+      <c r="C131" s="8" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="3">
+      <c r="A132" s="16">
         <v>130</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C132" s="9" t="s">
+      <c r="C132" s="8" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="3">
+      <c r="A133" s="14">
         <v>131</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C133" s="9" t="s">
+      <c r="C133" s="8" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="3">
+      <c r="A134" s="16">
         <v>132</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C134" s="9" t="s">
+      <c r="C134" s="8" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="3">
+      <c r="A135" s="14">
         <v>133</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C135" s="9" t="s">
+      <c r="C135" s="8" t="s">
         <v>287</v>
       </c>
     </row>

</xml_diff>